<commit_message>
Debug of file parser on preprocessed documents
</commit_message>
<xml_diff>
--- a/dossier_test/Etablissement4.xlsx
+++ b/dossier_test/Etablissement4.xlsx
@@ -1,21 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\sources\stat-generator\dossier_test\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36B0DBF7-C9DF-4034-9A6C-2395434257A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{8D6E54D3-8B50-493F-9E44-A06AFC535553}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="29070" windowHeight="16500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -364,6 +360,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" t="s">

</xml_diff>